<commit_message>
Fixed Board Outline Layer and Added digikey PNs to BOM
</commit_message>
<xml_diff>
--- a/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20104304-5AC0-4384-ACBD-40881CB403B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE54C20B-8719-4545-987A-D07E8ED95AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{7DCF6DCC-F933-41E2-93DB-2CAC20410EBB}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{77F1267C-2C76-402E-A719-CBB2675FE015}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -59,12 +56,12 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Supplier Part Number 1</t>
+  </si>
+  <si>
     <t>100nF</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>C1, C2, C3, C78, C84</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
     <t>CAP 100nF 16V X7R 0402</t>
   </si>
   <si>
+    <t>490-4759-1-ND</t>
+  </si>
+  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -83,6 +83,9 @@
     <t>CAP 10nF 50V X7R 0402</t>
   </si>
   <si>
+    <t>490-6351-1-ND</t>
+  </si>
+  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>CAP 4.7uF 6.3V X5R 0402</t>
   </si>
   <si>
+    <t>490-5915-1-ND</t>
+  </si>
+  <si>
     <t>470nF</t>
   </si>
   <si>
@@ -104,6 +110,9 @@
     <t>CAP 470nF 6.3V X5R 0201</t>
   </si>
   <si>
+    <t>490-10409-1-ND</t>
+  </si>
+  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -116,6 +125,9 @@
     <t>CAP 47uF 6.3V X5R 0805</t>
   </si>
   <si>
+    <t>1276-1852-1-ND</t>
+  </si>
+  <si>
     <t>100uF</t>
   </si>
   <si>
@@ -128,12 +140,18 @@
     <t>CAP 100uF 6.3V X5R 1210</t>
   </si>
   <si>
+    <t>1276-1092-1-ND</t>
+  </si>
+  <si>
     <t>C66, C67, C68, C69</t>
   </si>
   <si>
     <t>CAP 100nF 6.3V X5R 0201</t>
   </si>
   <si>
+    <t>490-3167-1-ND</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -146,6 +164,9 @@
     <t>CAP 10uF 10V X5R 0603</t>
   </si>
   <si>
+    <t>490-10474-1-ND</t>
+  </si>
+  <si>
     <t>39pF</t>
   </si>
   <si>
@@ -155,6 +176,9 @@
     <t>CAP 39pF 50V C0G 0402</t>
   </si>
   <si>
+    <t>399-C0402C390J5GAC7867CT-ND</t>
+  </si>
+  <si>
     <t>22uF</t>
   </si>
   <si>
@@ -164,6 +188,9 @@
     <t>CAP 22uF 25V X5R 0805</t>
   </si>
   <si>
+    <t>490-10749-1-ND</t>
+  </si>
+  <si>
     <t>120@100MHZ</t>
   </si>
   <si>
@@ -176,6 +203,9 @@
     <t>FERRITE BEAD 120 OHM 0402</t>
   </si>
   <si>
+    <t>490-9656-1-ND</t>
+  </si>
+  <si>
     <t>LSHM-150-04.0-L-DV-A-S-K-TR</t>
   </si>
   <si>
@@ -188,6 +218,9 @@
     <t>CONN LSHM-150-04.0-L-DV-A-S-K-TR</t>
   </si>
   <si>
+    <t>SAM9033CT-ND</t>
+  </si>
+  <si>
     <t>LSHM-130-04.0-L-DV-A-S-K-TR</t>
   </si>
   <si>
@@ -200,6 +233,9 @@
     <t>CONN LSHM-130-04.0-L-DV-A-S-K-TR</t>
   </si>
   <si>
+    <t>SAM9034CT-ND</t>
+  </si>
+  <si>
     <t>1uH</t>
   </si>
   <si>
@@ -212,6 +248,9 @@
     <t>IND 1uH 5.5A 32 MOHM 1210</t>
   </si>
   <si>
+    <t>118-SRP3212-1R0MCT-ND</t>
+  </si>
+  <si>
     <t>DMN62D0UW</t>
   </si>
   <si>
@@ -224,6 +263,9 @@
     <t>NMOS DMN62D0UW</t>
   </si>
   <si>
+    <t>DMN62D0UW-7DICT-ND</t>
+  </si>
+  <si>
     <t>100</t>
   </si>
   <si>
@@ -236,6 +278,9 @@
     <t>RES 100 OHM 1% 1/20W 0201</t>
   </si>
   <si>
+    <t>311-100MCT-ND</t>
+  </si>
+  <si>
     <t>4.7K</t>
   </si>
   <si>
@@ -245,6 +290,9 @@
     <t>RES 4.7K OHM 1% 1/20W 0201</t>
   </si>
   <si>
+    <t>311-4.70KMTR-ND</t>
+  </si>
+  <si>
     <t>240</t>
   </si>
   <si>
@@ -254,6 +302,9 @@
     <t>RES 240 OHM 1% 1/16W 0402</t>
   </si>
   <si>
+    <t>311-240LRTR-ND</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
@@ -263,6 +314,9 @@
     <t>RES 33 OHM 1% 1/20W 0201</t>
   </si>
   <si>
+    <t>RMCF0201FT33R0CT-ND</t>
+  </si>
+  <si>
     <t>1K</t>
   </si>
   <si>
@@ -272,6 +326,9 @@
     <t>RES 1K OHM 1% 1/10W 0402</t>
   </si>
   <si>
+    <t>311-1.00KLRCT-ND</t>
+  </si>
+  <si>
     <t>82</t>
   </si>
   <si>
@@ -281,6 +338,9 @@
     <t>RES 82 OHM 1% 1/16W 0402</t>
   </si>
   <si>
+    <t>311-82LRCT-ND</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
@@ -290,6 +350,9 @@
     <t>RES 100K OHM 1% 1/10W 0402</t>
   </si>
   <si>
+    <t>311-100KLRCT-ND</t>
+  </si>
+  <si>
     <t>66.5k</t>
   </si>
   <si>
@@ -299,6 +362,9 @@
     <t>RES 66.5K OHM 1% 1/16W 0402</t>
   </si>
   <si>
+    <t>YAG3209CT-ND</t>
+  </si>
+  <si>
     <t>124k</t>
   </si>
   <si>
@@ -308,6 +374,9 @@
     <t>RES 124K OHM 1% 1/10W 0402</t>
   </si>
   <si>
+    <t>311-124KLRCT-ND</t>
+  </si>
+  <si>
     <t>200K</t>
   </si>
   <si>
@@ -317,6 +386,9 @@
     <t>RES 200K OHM 1% 1/16W 0402</t>
   </si>
   <si>
+    <t>311-200KLRCT-ND</t>
+  </si>
+  <si>
     <t>0.01</t>
   </si>
   <si>
@@ -329,6 +401,9 @@
     <t>RES 0.01 OHM 1% 1/4W 0603</t>
   </si>
   <si>
+    <t>408-1404-1-ND</t>
+  </si>
+  <si>
     <t>140k</t>
   </si>
   <si>
@@ -338,12 +413,12 @@
     <t>RES 140K OHM 1% 1/10W 0402</t>
   </si>
   <si>
+    <t>YAG2978CT-ND</t>
+  </si>
+  <si>
     <t>IC FPGA XC7A50T-2CSG325C</t>
   </si>
   <si>
-    <t>Artix-7 FPGA, 150 User I/Os, 4 GTP, 324-Ball BGA, Speed Grade 2, Commercial Grade, Pb-Free</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -362,6 +437,9 @@
     <t>IC FLASH MX25U6432FZNI02</t>
   </si>
   <si>
+    <t>1092-MX25U6432FZNI02-ND</t>
+  </si>
+  <si>
     <t>TXB0104RUTR</t>
   </si>
   <si>
@@ -374,12 +452,12 @@
     <t>IC TRNSLTR TXB0104RUTR</t>
   </si>
   <si>
+    <t>296-25888-1-ND</t>
+  </si>
+  <si>
     <t>IC DDR3 MT41K64M16JT-15E</t>
   </si>
   <si>
-    <t>1Gb DDR3-1333 SDRAM, 64Mb x 16, 1.5ns, 1.35V, 0 to 95 degC, 96-Ball FBGA, Pb-Free</t>
-  </si>
-  <si>
     <t>U4, U5</t>
   </si>
   <si>
@@ -398,6 +476,9 @@
     <t>IC SWITCH LOAD SIP32508</t>
   </si>
   <si>
+    <t>SIP32508DT-T1-GE3CT-ND</t>
+  </si>
+  <si>
     <t>LD57100JR</t>
   </si>
   <si>
@@ -410,6 +491,9 @@
     <t>IC LDO LD57100JR</t>
   </si>
   <si>
+    <t>497-LD57100JRCT-ND</t>
+  </si>
+  <si>
     <t>TPS62A01</t>
   </si>
   <si>
@@ -422,6 +506,9 @@
     <t>IC BUCK TPS62A01</t>
   </si>
   <si>
+    <t>595-TPS62A01DRLR</t>
+  </si>
+  <si>
     <t>TPS62A02</t>
   </si>
   <si>
@@ -429,6 +516,15 @@
   </si>
   <si>
     <t>IC BUCK TPS62A02</t>
+  </si>
+  <si>
+    <t>595-TPS62A02DRLR</t>
+  </si>
+  <si>
+    <t>557-2010-1-ND</t>
+  </si>
+  <si>
+    <t>122-2193-ND</t>
   </si>
 </sst>
 </file>
@@ -804,14 +900,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15752CCE-FDE5-4E46-A079-37C27A2C72F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221A2809-BD51-4F16-BF10-EF60A7B482D7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -847,11 +946,11 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,97 +958,99 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E3" s="1">
         <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1">
         <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1">
         <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="1">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1">
         <v>5</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1">
         <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,555 +1058,579 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1">
         <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1">
         <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="1">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1">
         <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1">
         <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="1">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1">
         <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="1">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1">
         <v>2</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="1">
+        <v>63</v>
+      </c>
+      <c r="E14" s="1">
         <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="1">
+        <v>68</v>
+      </c>
+      <c r="E15" s="1">
         <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="1">
+        <v>73</v>
+      </c>
+      <c r="E16" s="1">
         <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="1">
+        <v>78</v>
+      </c>
+      <c r="E17" s="1">
         <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1">
         <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="1">
+        <v>86</v>
+      </c>
+      <c r="E19" s="1">
         <v>2</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="1">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1">
         <v>22</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="1">
+        <v>94</v>
+      </c>
+      <c r="E21" s="1">
         <v>2</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="1">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1">
         <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="1">
         <v>7</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="1">
-        <v>7</v>
+      <c r="F23" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="C24" s="2" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="1">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1">
         <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="1">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1">
         <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="1">
+        <v>114</v>
+      </c>
+      <c r="E26" s="1">
         <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="1">
+        <v>119</v>
+      </c>
+      <c r="E27" s="1">
         <v>5</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="1">
+        <v>123</v>
+      </c>
+      <c r="E28" s="1">
         <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="1">
+        <v>125</v>
+      </c>
+      <c r="E29" s="1">
         <v>1</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="C30" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="1">
+        <v>131</v>
+      </c>
+      <c r="E30" s="1">
         <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="C31" s="2" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="1">
+        <v>136</v>
+      </c>
+      <c r="E31" s="1">
         <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" s="1">
+        <v>138</v>
+      </c>
+      <c r="E32" s="1">
         <v>2</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="1">
+        <v>144</v>
+      </c>
+      <c r="E33" s="1">
         <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C34" s="2" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="1">
+        <v>149</v>
+      </c>
+      <c r="E34" s="1">
         <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="1">
+        <v>154</v>
+      </c>
+      <c r="E35" s="1">
         <v>2</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="C36" s="2" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="1">
+        <v>158</v>
+      </c>
+      <c r="E36" s="1">
         <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pulled back mounting hole copper from board edge
</commit_message>
<xml_diff>
--- a/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE54C20B-8719-4545-987A-D07E8ED95AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07B5C3F4-63B8-4260-B69B-20CF674A7177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{77F1267C-2C76-402E-A719-CBB2675FE015}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{CC651520-664A-4A64-8BCF-0CA4AC035E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="160">
   <si>
     <t>Comment</t>
   </si>
@@ -519,12 +519,6 @@
   </si>
   <si>
     <t>595-TPS62A02DRLR</t>
-  </si>
-  <si>
-    <t>557-2010-1-ND</t>
-  </si>
-  <si>
-    <t>122-2193-ND</t>
   </si>
 </sst>
 </file>
@@ -900,12 +894,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221A2809-BD51-4F16-BF10-EF60A7B482D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1D22FD-8939-45E8-BA48-2E8416BF4BDB}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1489,9 +1481,7 @@
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -1549,9 +1539,7 @@
       <c r="E32" s="1">
         <v>2</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">

</xml_diff>

<commit_message>
Added Connector Silkscreen RefDes and Gerbered out
</commit_message>
<xml_diff>
--- a/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/The Next Generation/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07B5C3F4-63B8-4260-B69B-20CF674A7177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B085F888-1594-4A06-A558-7B9FB9FAA18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{CC651520-664A-4A64-8BCF-0CA4AC035E2B}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{5461D050-A4BF-450D-B5C1-57397EF8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1D22FD-8939-45E8-BA48-2E8416BF4BDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09B0F29-2945-4363-96F1-F902566E2995}">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>